<commit_message>
Metodos de asignación y relacion de llave foranea
</commit_message>
<xml_diff>
--- a/DepreciationDBApp.Presentation/bin/Debug/net5.0-windows/Reporte.xlsx
+++ b/DepreciationDBApp.Presentation/bin/Debug/net5.0-windows/Reporte.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R37fa4fcd6fe34ec7"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R40cb1de085284761"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Nombre del Activo</x:t>
   </x:si>
@@ -38,13 +38,16 @@
     <x:t>Descripción</x:t>
   </x:si>
   <x:si>
-    <x:t>Teléfono</x:t>
+    <x:t>Pantalla led 4K de 55 pulgadas con HDR+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Televisor</x:t>
   </x:si>
   <x:si>
     <x:t>Kevin</x:t>
   </x:si>
   <x:si>
-    <x:t>8W1mFd1s</x:t>
+    <x:t>iCeKeFuq</x:t>
   </x:si>
   <x:si>
     <x:t>001</x:t>
@@ -457,16 +460,16 @@
     </x:row>
     <x:row r="3">
       <x:c r="B3" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C3" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D3" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -479,7 +482,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C8" s="6">
-        <x:v>15000</x:v>
+        <x:v>8500</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
@@ -487,14 +490,16 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C9" s="6">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="B10" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C10" s="6"/>
+      <x:c r="C10" s="6" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
 </x:worksheet>

</xml_diff>